<commit_message>
QCADOOCLS-7404 Fixed typo in operation import schema.
</commit_message>
<xml_diff>
--- a/mes-plugins/mes-plugins-technologies/src/main/resources/technologies/public/resources/operationImportSchema_de.xlsx
+++ b/mes-plugins/mes-plugins-technologies/src/main/resources/technologies/public/resources/operationImportSchema_de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/qcadoo-src/mes/mes-plugins/mes-plugins-technologies/src/main/resources/technologies/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BD8E30-DECB-8D4A-A5B5-9697024E244C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44E6412-550B-0E4A-8759-5B65B4FA0697}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>TPZ</t>
-  </si>
-  <si>
-    <t>TPJ</t>
   </si>
   <si>
     <t>Number</t>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>TJ</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,37 +1085,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DF Some fixes in import files.
</commit_message>
<xml_diff>
--- a/mes-plugins/mes-plugins-technologies/src/main/resources/technologies/public/resources/operationImportSchema_de.xlsx
+++ b/mes-plugins/mes-plugins-technologies/src/main/resources/technologies/public/resources/operationImportSchema_de.xlsx
@@ -73,12 +73,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -91,13 +97,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -106,31 +112,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -147,13 +153,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -173,6 +179,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -372,17 +379,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -410,10 +417,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -661,12 +668,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -953,7 +960,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -981,10 +988,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1235,7 +1242,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1244,8 +1251,7 @@
     <col min="1" max="3" width="16.8516" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.8516" style="1" customWidth="1"/>
     <col min="5" max="10" width="16.8516" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8516" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -1279,813 +1285,750 @@
       <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" s="3"/>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" ht="16" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" ht="16" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" ht="16" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" ht="16" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" ht="16" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" ht="16" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" ht="16" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" ht="16" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" ht="16" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" ht="16" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" ht="16" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" ht="16" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" ht="16" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" ht="16" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" ht="16" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" ht="16" customHeight="1">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" ht="16" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" ht="16" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" ht="16" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" ht="16" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32" ht="16" customHeight="1">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" ht="16" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" ht="16" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" ht="16" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" ht="16" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37" ht="16" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" ht="16" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="39" ht="16" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="40" ht="16" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
     </row>
     <row r="41" ht="16" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" ht="16" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
     </row>
     <row r="43" ht="16" customHeight="1">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
     </row>
     <row r="44" ht="16" customHeight="1">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
     </row>
     <row r="45" ht="16" customHeight="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
     </row>
     <row r="46" ht="16" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
     </row>
     <row r="47" ht="16" customHeight="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
     </row>
     <row r="48" ht="16" customHeight="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
     </row>
     <row r="49" ht="16" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
     </row>
     <row r="50" ht="16" customHeight="1">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
     </row>
     <row r="51" ht="16" customHeight="1">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
     </row>
     <row r="52" ht="16" customHeight="1">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53" ht="16" customHeight="1">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54" ht="16" customHeight="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
     </row>
     <row r="55" ht="16" customHeight="1">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
     </row>
     <row r="56" ht="16" customHeight="1">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
     </row>
     <row r="57" ht="16" customHeight="1">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
     </row>
     <row r="58" ht="16" customHeight="1">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
     </row>
     <row r="59" ht="16" customHeight="1">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
     </row>
     <row r="60" ht="16" customHeight="1">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
     </row>
     <row r="61" ht="16" customHeight="1">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
     </row>
     <row r="62" ht="16" customHeight="1">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
     </row>
     <row r="63" ht="16" customHeight="1">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>